<commit_message>
Implemented part heapsort. Introsort has trouble sorting 50% sorted array.
</commit_message>
<xml_diff>
--- a/sprawozdanie/intro_wykres.xlsx
+++ b/sprawozdanie/intro_wykres.xlsx
@@ -8,14 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kuba\Desktop\STUDIA\Semestr 4\PAMSI\C++\Projekt 1 - Sortowanie\sprawozdanie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8279DD4-4C70-4FE2-BDFF-D0823717D34D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{045FDCFD-9F0E-4F07-948B-82CE69316BBE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27630" windowHeight="11565" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="quick_wykres" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -94,10 +101,10 @@
     <t>100.00% OF ARRAY IS SORTED, BUT IT'S REVERSED</t>
   </si>
   <si>
-    <t>AVERAGE 100R</t>
+    <t>End of results</t>
   </si>
   <si>
-    <t>End of results</t>
+    <t>AVERAGE 100</t>
   </si>
 </sst>
 </file>
@@ -797,19 +804,19 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1.04</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.63</c:v>
+                  <c:v>6.77</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>23.13</c:v>
+                  <c:v>14.43</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>139.36000000000001</c:v>
+                  <c:v>84.97</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>299.35000000000002</c:v>
+                  <c:v>180.23</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -846,16 +853,16 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.02</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>22.29</c:v>
+                  <c:v>14.33</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>132.49</c:v>
+                  <c:v>84.1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>284.01</c:v>
+                  <c:v>178.77</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -889,19 +896,19 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.27</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.61</c:v>
+                  <c:v>9.64</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20.83</c:v>
+                  <c:v>20.81</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>123.26</c:v>
+                  <c:v>124.15</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>263.25</c:v>
+                  <c:v>248.84</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -935,19 +942,19 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0.9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9</c:v>
+                  <c:v>5.87</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>19.68</c:v>
+                  <c:v>12.78</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>113.65</c:v>
+                  <c:v>77.2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>243.83</c:v>
+                  <c:v>165.36</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -981,19 +988,19 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0.49</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.26</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>18.18</c:v>
+                  <c:v>12.99</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>104.81</c:v>
+                  <c:v>81.209999999999994</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>221.91</c:v>
+                  <c:v>176.89</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1027,19 +1034,19 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.15</c:v>
+                  <c:v>4.07</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>18.02</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>102.97</c:v>
+                  <c:v>64.540000000000006</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>217.28</c:v>
+                  <c:v>144.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1075,19 +1082,19 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.0399999999999991</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>18.03</c:v>
+                  <c:v>9.1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>102.26</c:v>
+                  <c:v>57.24</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>216.41</c:v>
+                  <c:v>127.01</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1123,19 +1130,19 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.01</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17.38</c:v>
+                  <c:v>7.03</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>99.96</c:v>
+                  <c:v>44.63</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>210.08</c:v>
+                  <c:v>95.69</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2088,15 +2095,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>366031</xdr:colOff>
+      <xdr:colOff>366032</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>3401</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>13607</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>13607</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>122464</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>81643</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2424,12 +2431,12 @@
   <dimension ref="A1:H242"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="AI18" sqref="AI18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="8" max="8" width="9.140625" style="1"/>
+    <col min="8" max="8" width="10" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -2451,7 +2458,8 @@
         <v>10000</v>
       </c>
       <c r="H2" s="1">
-        <v>1.04</v>
+        <f>B3</f>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -2459,13 +2467,14 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>1.04</v>
+        <v>1</v>
       </c>
       <c r="G3">
         <v>50000</v>
       </c>
       <c r="H3" s="1">
-        <v>10.63</v>
+        <f>B9</f>
+        <v>6.77</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -2479,7 +2488,8 @@
         <v>100000</v>
       </c>
       <c r="H4" s="1">
-        <v>23.13</v>
+        <f>B15</f>
+        <v>14.43</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -2487,13 +2497,14 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G5">
         <v>500000</v>
       </c>
       <c r="H5" s="1">
-        <v>139.36000000000001</v>
+        <f>B21</f>
+        <v>84.97</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -2501,7 +2512,8 @@
         <v>1000000</v>
       </c>
       <c r="H6" s="1">
-        <v>299.35000000000002</v>
+        <f>B27</f>
+        <v>180.23</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -2519,7 +2531,7 @@
         <v>4</v>
       </c>
       <c r="B9">
-        <v>10.63</v>
+        <v>6.77</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -2527,7 +2539,7 @@
         <v>5</v>
       </c>
       <c r="B10">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -2535,7 +2547,7 @@
         <v>6</v>
       </c>
       <c r="B11">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -2553,7 +2565,7 @@
         <v>4</v>
       </c>
       <c r="B15">
-        <v>23.13</v>
+        <v>14.43</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -2561,7 +2573,7 @@
         <v>5</v>
       </c>
       <c r="B16">
-        <v>23</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -2569,7 +2581,7 @@
         <v>6</v>
       </c>
       <c r="B17">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -2587,7 +2599,7 @@
         <v>4</v>
       </c>
       <c r="B21">
-        <v>139.36000000000001</v>
+        <v>84.97</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -2595,7 +2607,7 @@
         <v>5</v>
       </c>
       <c r="B22">
-        <v>137</v>
+        <v>83</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -2603,7 +2615,7 @@
         <v>6</v>
       </c>
       <c r="B23">
-        <v>147</v>
+        <v>92</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -2621,7 +2633,7 @@
         <v>4</v>
       </c>
       <c r="B27">
-        <v>299.35000000000002</v>
+        <v>180.23</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -2629,7 +2641,7 @@
         <v>5</v>
       </c>
       <c r="B28">
-        <v>292</v>
+        <v>176</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -2637,7 +2649,7 @@
         <v>6</v>
       </c>
       <c r="B29">
-        <v>323</v>
+        <v>189</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -2653,6 +2665,7 @@
         <v>3</v>
       </c>
       <c r="H32" s="1">
+        <f>B33</f>
         <v>1</v>
       </c>
     </row>
@@ -2664,7 +2677,8 @@
         <v>1</v>
       </c>
       <c r="H33" s="1">
-        <v>10.02</v>
+        <f>B39</f>
+        <v>6.5</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -2675,7 +2689,8 @@
         <v>1</v>
       </c>
       <c r="H34" s="1">
-        <v>22.29</v>
+        <f>B45</f>
+        <v>14.33</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -2686,12 +2701,14 @@
         <v>1</v>
       </c>
       <c r="H35" s="1">
-        <v>132.49</v>
+        <f>B51</f>
+        <v>84.1</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H36" s="1">
-        <v>284.01</v>
+        <f>B57</f>
+        <v>178.77</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -2709,7 +2726,7 @@
         <v>4</v>
       </c>
       <c r="B39">
-        <v>10.02</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -2717,7 +2734,7 @@
         <v>5</v>
       </c>
       <c r="B40">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -2725,7 +2742,7 @@
         <v>6</v>
       </c>
       <c r="B41">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -2743,7 +2760,7 @@
         <v>4</v>
       </c>
       <c r="B45">
-        <v>22.29</v>
+        <v>14.33</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -2751,7 +2768,7 @@
         <v>5</v>
       </c>
       <c r="B46">
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -2759,7 +2776,7 @@
         <v>6</v>
       </c>
       <c r="B47">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
@@ -2777,7 +2794,7 @@
         <v>4</v>
       </c>
       <c r="B51">
-        <v>132.49</v>
+        <v>84.1</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
@@ -2785,7 +2802,7 @@
         <v>5</v>
       </c>
       <c r="B52">
-        <v>130</v>
+        <v>81</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
@@ -2793,7 +2810,7 @@
         <v>6</v>
       </c>
       <c r="B53">
-        <v>140</v>
+        <v>92</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
@@ -2811,7 +2828,7 @@
         <v>4</v>
       </c>
       <c r="B57">
-        <v>284.01</v>
+        <v>178.77</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
@@ -2819,7 +2836,7 @@
         <v>5</v>
       </c>
       <c r="B58">
-        <v>279</v>
+        <v>173</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
@@ -2827,7 +2844,7 @@
         <v>6</v>
       </c>
       <c r="B59">
-        <v>291</v>
+        <v>191</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
@@ -2843,7 +2860,8 @@
         <v>3</v>
       </c>
       <c r="H62" s="1">
-        <v>1</v>
+        <f>B63</f>
+        <v>1.27</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
@@ -2851,10 +2869,11 @@
         <v>4</v>
       </c>
       <c r="B63">
-        <v>1</v>
+        <v>1.27</v>
       </c>
       <c r="H63" s="1">
-        <v>9.61</v>
+        <f>B69</f>
+        <v>9.64</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
@@ -2865,7 +2884,8 @@
         <v>1</v>
       </c>
       <c r="H64" s="1">
-        <v>20.83</v>
+        <f>B75</f>
+        <v>20.81</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
@@ -2873,15 +2893,17 @@
         <v>6</v>
       </c>
       <c r="B65">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H65" s="1">
-        <v>123.26</v>
+        <f>B81</f>
+        <v>124.15</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H66" s="1">
-        <v>263.25</v>
+        <f>B87</f>
+        <v>248.84</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
@@ -2899,7 +2921,7 @@
         <v>4</v>
       </c>
       <c r="B69">
-        <v>9.61</v>
+        <v>9.64</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
@@ -2907,7 +2929,7 @@
         <v>5</v>
       </c>
       <c r="B70">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
@@ -2915,7 +2937,7 @@
         <v>6</v>
       </c>
       <c r="B71">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
@@ -2933,7 +2955,7 @@
         <v>4</v>
       </c>
       <c r="B75">
-        <v>20.83</v>
+        <v>20.81</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
@@ -2941,7 +2963,7 @@
         <v>5</v>
       </c>
       <c r="B76">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
@@ -2949,7 +2971,7 @@
         <v>6</v>
       </c>
       <c r="B77">
-        <v>22</v>
+        <v>33</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
@@ -2967,7 +2989,7 @@
         <v>4</v>
       </c>
       <c r="B81">
-        <v>123.26</v>
+        <v>124.15</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
@@ -2975,7 +2997,7 @@
         <v>5</v>
       </c>
       <c r="B82">
-        <v>120</v>
+        <v>83</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
@@ -2983,7 +3005,7 @@
         <v>6</v>
       </c>
       <c r="B83">
-        <v>131</v>
+        <v>185</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
@@ -3001,7 +3023,7 @@
         <v>4</v>
       </c>
       <c r="B87">
-        <v>263.25</v>
+        <v>248.84</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
@@ -3009,7 +3031,7 @@
         <v>5</v>
       </c>
       <c r="B88">
-        <v>258</v>
+        <v>176</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
@@ -3017,7 +3039,7 @@
         <v>6</v>
       </c>
       <c r="B89">
-        <v>272</v>
+        <v>388</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
@@ -3033,7 +3055,8 @@
         <v>3</v>
       </c>
       <c r="H92" s="1">
-        <v>1</v>
+        <f>B93</f>
+        <v>0.9</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
@@ -3041,10 +3064,11 @@
         <v>4</v>
       </c>
       <c r="B93">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="H93" s="1">
-        <v>9</v>
+        <f>B99</f>
+        <v>5.87</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
@@ -3052,10 +3076,11 @@
         <v>5</v>
       </c>
       <c r="B94">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H94" s="1">
-        <v>19.68</v>
+        <f>B105</f>
+        <v>12.78</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
@@ -3066,12 +3091,14 @@
         <v>1</v>
       </c>
       <c r="H95" s="1">
-        <v>113.65</v>
+        <f>B111</f>
+        <v>77.2</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H96" s="1">
-        <v>243.83</v>
+        <f>B117</f>
+        <v>165.36</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
@@ -3089,7 +3116,7 @@
         <v>4</v>
       </c>
       <c r="B99">
-        <v>9</v>
+        <v>5.87</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
@@ -3097,7 +3124,7 @@
         <v>5</v>
       </c>
       <c r="B100">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
@@ -3105,7 +3132,7 @@
         <v>6</v>
       </c>
       <c r="B101">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
@@ -3123,7 +3150,7 @@
         <v>4</v>
       </c>
       <c r="B105">
-        <v>19.68</v>
+        <v>12.78</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
@@ -3131,7 +3158,7 @@
         <v>5</v>
       </c>
       <c r="B106">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
@@ -3139,7 +3166,7 @@
         <v>6</v>
       </c>
       <c r="B107">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
@@ -3157,7 +3184,7 @@
         <v>4</v>
       </c>
       <c r="B111">
-        <v>113.65</v>
+        <v>77.2</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
@@ -3165,7 +3192,7 @@
         <v>5</v>
       </c>
       <c r="B112">
-        <v>110</v>
+        <v>74</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
@@ -3173,7 +3200,7 @@
         <v>6</v>
       </c>
       <c r="B113">
-        <v>123</v>
+        <v>83</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
@@ -3191,7 +3218,7 @@
         <v>4</v>
       </c>
       <c r="B117">
-        <v>243.83</v>
+        <v>165.36</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
@@ -3199,7 +3226,7 @@
         <v>5</v>
       </c>
       <c r="B118">
-        <v>235</v>
+        <v>158</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
@@ -3207,7 +3234,7 @@
         <v>6</v>
       </c>
       <c r="B119">
-        <v>257</v>
+        <v>181</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
@@ -3223,7 +3250,8 @@
         <v>3</v>
       </c>
       <c r="H122" s="1">
-        <v>1</v>
+        <f>B123</f>
+        <v>0.49</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
@@ -3231,10 +3259,11 @@
         <v>4</v>
       </c>
       <c r="B123">
-        <v>1</v>
+        <v>0.49</v>
       </c>
       <c r="H123" s="1">
-        <v>8.26</v>
+        <f>B129</f>
+        <v>6</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
@@ -3242,10 +3271,11 @@
         <v>5</v>
       </c>
       <c r="B124">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H124" s="1">
-        <v>18.18</v>
+        <f>B135</f>
+        <v>12.99</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
@@ -3256,12 +3286,14 @@
         <v>1</v>
       </c>
       <c r="H125" s="1">
-        <v>104.81</v>
+        <f>B141</f>
+        <v>81.209999999999994</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H126" s="1">
-        <v>221.91</v>
+        <f>B147</f>
+        <v>176.89</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
@@ -3279,7 +3311,7 @@
         <v>4</v>
       </c>
       <c r="B129">
-        <v>8.26</v>
+        <v>6</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
@@ -3287,7 +3319,7 @@
         <v>5</v>
       </c>
       <c r="B130">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
@@ -3295,7 +3327,7 @@
         <v>6</v>
       </c>
       <c r="B131">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
@@ -3313,7 +3345,7 @@
         <v>4</v>
       </c>
       <c r="B135">
-        <v>18.18</v>
+        <v>12.99</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
@@ -3321,7 +3353,7 @@
         <v>5</v>
       </c>
       <c r="B136">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
@@ -3329,7 +3361,7 @@
         <v>6</v>
       </c>
       <c r="B137">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
@@ -3347,7 +3379,7 @@
         <v>4</v>
       </c>
       <c r="B141">
-        <v>104.81</v>
+        <v>81.209999999999994</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
@@ -3355,7 +3387,7 @@
         <v>5</v>
       </c>
       <c r="B142">
-        <v>103</v>
+        <v>79</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
@@ -3363,7 +3395,7 @@
         <v>6</v>
       </c>
       <c r="B143">
-        <v>110</v>
+        <v>85</v>
       </c>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.25">
@@ -3381,7 +3413,7 @@
         <v>4</v>
       </c>
       <c r="B147">
-        <v>221.91</v>
+        <v>176.89</v>
       </c>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.25">
@@ -3389,7 +3421,7 @@
         <v>5</v>
       </c>
       <c r="B148">
-        <v>218</v>
+        <v>172</v>
       </c>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.25">
@@ -3397,7 +3429,7 @@
         <v>6</v>
       </c>
       <c r="B149">
-        <v>234</v>
+        <v>183</v>
       </c>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.25">
@@ -3413,7 +3445,8 @@
         <v>3</v>
       </c>
       <c r="H152" s="1">
-        <v>1</v>
+        <f>B153</f>
+        <v>0</v>
       </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.25">
@@ -3421,10 +3454,11 @@
         <v>4</v>
       </c>
       <c r="B153">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H153" s="1">
-        <v>8.15</v>
+        <f>B159</f>
+        <v>4.07</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.25">
@@ -3432,10 +3466,11 @@
         <v>5</v>
       </c>
       <c r="B154">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H154" s="1">
-        <v>18.02</v>
+        <f>B165</f>
+        <v>10</v>
       </c>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.25">
@@ -3443,15 +3478,17 @@
         <v>6</v>
       </c>
       <c r="B155">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H155" s="1">
-        <v>102.97</v>
+        <f>B171</f>
+        <v>64.540000000000006</v>
       </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H156" s="1">
-        <v>217.28</v>
+        <f>B177</f>
+        <v>144.25</v>
       </c>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.25">
@@ -3469,7 +3506,7 @@
         <v>4</v>
       </c>
       <c r="B159">
-        <v>8.15</v>
+        <v>4.07</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.25">
@@ -3477,7 +3514,7 @@
         <v>5</v>
       </c>
       <c r="B160">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
@@ -3485,7 +3522,7 @@
         <v>6</v>
       </c>
       <c r="B161">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
@@ -3503,7 +3540,7 @@
         <v>4</v>
       </c>
       <c r="B165">
-        <v>18.02</v>
+        <v>10</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
@@ -3511,7 +3548,7 @@
         <v>5</v>
       </c>
       <c r="B166">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
@@ -3519,7 +3556,7 @@
         <v>6</v>
       </c>
       <c r="B167">
-        <v>19</v>
+        <v>10</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
@@ -3537,7 +3574,7 @@
         <v>4</v>
       </c>
       <c r="B171">
-        <v>102.97</v>
+        <v>64.540000000000006</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
@@ -3545,7 +3582,7 @@
         <v>5</v>
       </c>
       <c r="B172">
-        <v>101</v>
+        <v>64</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
@@ -3553,7 +3590,7 @@
         <v>6</v>
       </c>
       <c r="B173">
-        <v>111</v>
+        <v>67</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
@@ -3571,7 +3608,7 @@
         <v>4</v>
       </c>
       <c r="B177">
-        <v>217.28</v>
+        <v>144.25</v>
       </c>
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.25">
@@ -3579,7 +3616,7 @@
         <v>5</v>
       </c>
       <c r="B178">
-        <v>214</v>
+        <v>142</v>
       </c>
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.25">
@@ -3587,7 +3624,7 @@
         <v>6</v>
       </c>
       <c r="B179">
-        <v>232</v>
+        <v>149</v>
       </c>
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.25">
@@ -3603,7 +3640,8 @@
         <v>3</v>
       </c>
       <c r="H182" s="1">
-        <v>1</v>
+        <f>B183</f>
+        <v>0</v>
       </c>
     </row>
     <row r="183" spans="1:8" x14ac:dyDescent="0.25">
@@ -3611,10 +3649,11 @@
         <v>4</v>
       </c>
       <c r="B183">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H183" s="1">
-        <v>8.0399999999999991</v>
+        <f>B189</f>
+        <v>4</v>
       </c>
     </row>
     <row r="184" spans="1:8" x14ac:dyDescent="0.25">
@@ -3622,10 +3661,11 @@
         <v>5</v>
       </c>
       <c r="B184">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H184" s="1">
-        <v>18.03</v>
+        <f>B195</f>
+        <v>9.1</v>
       </c>
     </row>
     <row r="185" spans="1:8" x14ac:dyDescent="0.25">
@@ -3633,15 +3673,17 @@
         <v>6</v>
       </c>
       <c r="B185">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H185" s="1">
-        <v>102.26</v>
+        <f>B201</f>
+        <v>57.24</v>
       </c>
     </row>
     <row r="186" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H186" s="1">
-        <v>216.41</v>
+        <f>B207</f>
+        <v>127.01</v>
       </c>
     </row>
     <row r="187" spans="1:8" x14ac:dyDescent="0.25">
@@ -3659,7 +3701,7 @@
         <v>4</v>
       </c>
       <c r="B189">
-        <v>8.0399999999999991</v>
+        <v>4</v>
       </c>
     </row>
     <row r="190" spans="1:8" x14ac:dyDescent="0.25">
@@ -3667,7 +3709,7 @@
         <v>5</v>
       </c>
       <c r="B190">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="191" spans="1:8" x14ac:dyDescent="0.25">
@@ -3675,7 +3717,7 @@
         <v>6</v>
       </c>
       <c r="B191">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
@@ -3693,7 +3735,7 @@
         <v>4</v>
       </c>
       <c r="B195">
-        <v>18.03</v>
+        <v>9.1</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
@@ -3701,7 +3743,7 @@
         <v>5</v>
       </c>
       <c r="B196">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
@@ -3709,7 +3751,7 @@
         <v>6</v>
       </c>
       <c r="B197">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
@@ -3727,7 +3769,7 @@
         <v>4</v>
       </c>
       <c r="B201">
-        <v>102.26</v>
+        <v>57.24</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
@@ -3735,7 +3777,7 @@
         <v>5</v>
       </c>
       <c r="B202">
-        <v>101</v>
+        <v>57</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
@@ -3743,7 +3785,7 @@
         <v>6</v>
       </c>
       <c r="B203">
-        <v>111</v>
+        <v>61</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
@@ -3761,7 +3803,7 @@
         <v>4</v>
       </c>
       <c r="B207">
-        <v>216.41</v>
+        <v>127.01</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
@@ -3769,7 +3811,7 @@
         <v>5</v>
       </c>
       <c r="B208">
-        <v>212</v>
+        <v>126</v>
       </c>
     </row>
     <row r="209" spans="1:8" x14ac:dyDescent="0.25">
@@ -3777,7 +3819,7 @@
         <v>6</v>
       </c>
       <c r="B209">
-        <v>233</v>
+        <v>129</v>
       </c>
     </row>
     <row r="211" spans="1:8" x14ac:dyDescent="0.25">
@@ -3785,7 +3827,7 @@
         <v>23</v>
       </c>
       <c r="H211" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="212" spans="1:8" x14ac:dyDescent="0.25">
@@ -3793,7 +3835,8 @@
         <v>3</v>
       </c>
       <c r="H212" s="1">
-        <v>1</v>
+        <f>B213</f>
+        <v>0</v>
       </c>
     </row>
     <row r="213" spans="1:8" x14ac:dyDescent="0.25">
@@ -3801,10 +3844,11 @@
         <v>4</v>
       </c>
       <c r="B213">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H213" s="1">
-        <v>8.01</v>
+        <f>B219</f>
+        <v>3</v>
       </c>
     </row>
     <row r="214" spans="1:8" x14ac:dyDescent="0.25">
@@ -3812,10 +3856,11 @@
         <v>5</v>
       </c>
       <c r="B214">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H214" s="1">
-        <v>17.38</v>
+        <f>B225</f>
+        <v>7.03</v>
       </c>
     </row>
     <row r="215" spans="1:8" x14ac:dyDescent="0.25">
@@ -3823,15 +3868,17 @@
         <v>6</v>
       </c>
       <c r="B215">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H215" s="1">
-        <v>99.96</v>
+        <f>B231</f>
+        <v>44.63</v>
       </c>
     </row>
     <row r="216" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H216" s="1">
-        <v>210.08</v>
+        <f>B237</f>
+        <v>95.69</v>
       </c>
     </row>
     <row r="217" spans="1:8" x14ac:dyDescent="0.25">
@@ -3849,7 +3896,7 @@
         <v>4</v>
       </c>
       <c r="B219">
-        <v>8.01</v>
+        <v>3</v>
       </c>
     </row>
     <row r="220" spans="1:8" x14ac:dyDescent="0.25">
@@ -3857,7 +3904,7 @@
         <v>5</v>
       </c>
       <c r="B220">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="221" spans="1:8" x14ac:dyDescent="0.25">
@@ -3865,7 +3912,7 @@
         <v>6</v>
       </c>
       <c r="B221">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="223" spans="1:8" x14ac:dyDescent="0.25">
@@ -3883,7 +3930,7 @@
         <v>4</v>
       </c>
       <c r="B225">
-        <v>17.38</v>
+        <v>7.03</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.25">
@@ -3891,7 +3938,7 @@
         <v>5</v>
       </c>
       <c r="B226">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.25">
@@ -3899,7 +3946,7 @@
         <v>6</v>
       </c>
       <c r="B227">
-        <v>19</v>
+        <v>8</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.25">
@@ -3917,7 +3964,7 @@
         <v>4</v>
       </c>
       <c r="B231">
-        <v>99.96</v>
+        <v>44.63</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.25">
@@ -3925,7 +3972,7 @@
         <v>5</v>
       </c>
       <c r="B232">
-        <v>97</v>
+        <v>44</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.25">
@@ -3933,7 +3980,7 @@
         <v>6</v>
       </c>
       <c r="B233">
-        <v>105</v>
+        <v>45</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.25">
@@ -3951,7 +3998,7 @@
         <v>4</v>
       </c>
       <c r="B237">
-        <v>210.08</v>
+        <v>95.69</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.25">
@@ -3959,7 +4006,7 @@
         <v>5</v>
       </c>
       <c r="B238">
-        <v>205</v>
+        <v>95</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.25">
@@ -3967,12 +4014,12 @@
         <v>6</v>
       </c>
       <c r="B239">
-        <v>229</v>
+        <v>97</v>
       </c>
     </row>
     <row r="242" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>